<commit_message>
neuste version von der excel-datei
</commit_message>
<xml_diff>
--- a/Dokumentation/Dokumentation_Projekt-Steuerung_Autonom-Fahrendes-Auto_cargroup03_After_9f32617dcf09bb7ac3d91f3f63ed8d08ef1232e2.xlsx
+++ b/Dokumentation/Dokumentation_Projekt-Steuerung_Autonom-Fahrendes-Auto_cargroup03_After_9f32617dcf09bb7ac3d91f3f63ed8d08ef1232e2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ESY_2324\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E0772B-6396-4E3B-B381-9D28177A480D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22531D4C-AE16-4041-B5AA-AAC6FCDB1F83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" tabRatio="500" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" tabRatio="500" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektüberblick" sheetId="1" r:id="rId1"/>
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="235">
   <si>
     <t>Projektstart:</t>
   </si>
@@ -1140,6 +1140,9 @@
   </si>
   <si>
     <t xml:space="preserve">Code von letzter Woche erweitert, für Rechtskurven </t>
+  </si>
+  <si>
+    <t>Sensor vorne eingabut und Programm geschrieben, nächste Woche weiter daran arbeiten</t>
   </si>
 </sst>
 </file>
@@ -1532,7 +1535,7 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1865,12 +1868,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -1879,36 +1915,6 @@
     </xf>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2419,14 +2425,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="126" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -2475,10 +2481,10 @@
       <c r="D7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="115" t="s">
+      <c r="E7" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="115"/>
+      <c r="F7" s="121"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2489,8 +2495,8 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="116"/>
+      <c r="E8" s="127"/>
+      <c r="F8" s="127"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
@@ -2501,8 +2507,8 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="117"/>
-      <c r="F9" s="117"/>
+      <c r="E9" s="128"/>
+      <c r="F9" s="128"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
@@ -2513,8 +2519,8 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="118"/>
-      <c r="F10" s="118"/>
+      <c r="E10" s="129"/>
+      <c r="F10" s="129"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2525,8 +2531,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="119"/>
-      <c r="F11" s="119"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="17"/>
@@ -2547,49 +2553,49 @@
       <c r="A15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="120"/>
-      <c r="C15" s="120"/>
-      <c r="D15" s="120"/>
-      <c r="E15" s="120"/>
-      <c r="F15" s="120"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="124"/>
+      <c r="D15" s="124"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="124"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="121"/>
-      <c r="C16" s="121"/>
-      <c r="D16" s="121"/>
-      <c r="E16" s="121"/>
-      <c r="F16" s="121"/>
+      <c r="B16" s="125"/>
+      <c r="C16" s="125"/>
+      <c r="D16" s="125"/>
+      <c r="E16" s="125"/>
+      <c r="F16" s="125"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="121"/>
-      <c r="C17" s="121"/>
-      <c r="D17" s="121"/>
-      <c r="E17" s="121"/>
-      <c r="F17" s="121"/>
+      <c r="B17" s="125"/>
+      <c r="C17" s="125"/>
+      <c r="D17" s="125"/>
+      <c r="E17" s="125"/>
+      <c r="F17" s="125"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="121"/>
-      <c r="C18" s="121"/>
-      <c r="D18" s="121"/>
-      <c r="E18" s="121"/>
-      <c r="F18" s="121"/>
+      <c r="B18" s="125"/>
+      <c r="C18" s="125"/>
+      <c r="D18" s="125"/>
+      <c r="E18" s="125"/>
+      <c r="F18" s="125"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="126"/>
-      <c r="C19" s="126"/>
-      <c r="D19" s="126"/>
-      <c r="E19" s="126"/>
-      <c r="F19" s="126"/>
+      <c r="B19" s="119"/>
+      <c r="C19" s="119"/>
+      <c r="D19" s="119"/>
+      <c r="E19" s="119"/>
+      <c r="F19" s="119"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
@@ -2602,64 +2608,74 @@
       <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="127" t="s">
+      <c r="A23" s="120" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="127"/>
-      <c r="C23" s="127"/>
-      <c r="D23" s="127"/>
-      <c r="E23" s="127"/>
-      <c r="F23" s="127"/>
+      <c r="B23" s="120"/>
+      <c r="C23" s="120"/>
+      <c r="D23" s="120"/>
+      <c r="E23" s="120"/>
+      <c r="F23" s="120"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="115" t="s">
+      <c r="A26" s="121" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="115"/>
-      <c r="C26" s="115"/>
-      <c r="D26" s="115" t="s">
+      <c r="B26" s="121"/>
+      <c r="C26" s="121"/>
+      <c r="D26" s="121" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="115"/>
-      <c r="F26" s="115"/>
+      <c r="E26" s="121"/>
+      <c r="F26" s="121"/>
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="123" t="s">
+      <c r="A27" s="116" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="123"/>
-      <c r="C27" s="123"/>
-      <c r="D27" s="128"/>
-      <c r="E27" s="128"/>
-      <c r="F27" s="128"/>
+      <c r="B27" s="116"/>
+      <c r="C27" s="116"/>
+      <c r="D27" s="122"/>
+      <c r="E27" s="122"/>
+      <c r="F27" s="122"/>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="122" t="s">
+      <c r="A28" s="115" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="122"/>
-      <c r="C28" s="122"/>
-      <c r="D28" s="123" t="s">
+      <c r="B28" s="115"/>
+      <c r="C28" s="115"/>
+      <c r="D28" s="116" t="s">
         <v>204</v>
       </c>
-      <c r="E28" s="123"/>
-      <c r="F28" s="123"/>
+      <c r="E28" s="116"/>
+      <c r="F28" s="116"/>
     </row>
     <row r="29" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="124" t="s">
+      <c r="A29" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="124"/>
-      <c r="C29" s="124"/>
-      <c r="D29" s="125"/>
-      <c r="E29" s="125"/>
-      <c r="F29" s="125"/>
+      <c r="B29" s="117"/>
+      <c r="C29" s="117"/>
+      <c r="D29" s="118"/>
+      <c r="E29" s="118"/>
+      <c r="F29" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="A29:C29"/>
@@ -2670,16 +2686,6 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2695,7 +2701,7 @@
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2707,11 +2713,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="131" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
     </row>
     <row r="3" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -2867,10 +2873,16 @@
         <v>233</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="105"/>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="40">
+        <v>45271</v>
+      </c>
+      <c r="B17" s="41">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="C17" s="114" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="41"/>
@@ -2969,7 +2981,7 @@
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:C21"/>
+      <selection activeCell="A18" sqref="A18:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2981,11 +2993,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="131" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
     </row>
     <row r="3" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -3152,10 +3164,16 @@
         <v>233</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="2"/>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="40">
+        <v>45271</v>
+      </c>
+      <c r="B18" s="41">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="41"/>
@@ -3319,29 +3337,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="126" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="130" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="129"/>
+      <c r="C3" s="130"/>
     </row>
     <row r="4" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="130" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="129"/>
+      <c r="C4" s="130"/>
     </row>
     <row r="5" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="129" t="s">
+      <c r="B5" s="130" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="129"/>
+      <c r="C5" s="130"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -3564,11 +3582,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="131" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="35"/>
@@ -3576,18 +3594,18 @@
       <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="131" t="s">
+      <c r="A3" s="132" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="131"/>
-      <c r="C3" s="131"/>
+      <c r="B3" s="132"/>
+      <c r="C3" s="132"/>
     </row>
     <row r="4" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="132" t="s">
+      <c r="A4" s="133" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="132"/>
-      <c r="C4" s="132"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="133"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
@@ -3839,7 +3857,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -3855,14 +3873,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="131" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
     </row>
     <row r="3" spans="1:6" s="43" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -4140,8 +4158,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4155,16 +4173,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="126" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
     </row>
     <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
@@ -4486,7 +4504,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="56">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F18" s="56">
         <v>2</v>
@@ -4794,7 +4812,7 @@
       </c>
       <c r="E35" s="49">
         <f>SUM(E10:E34)</f>
-        <v>10.25</v>
+        <v>12.25</v>
       </c>
       <c r="F35" s="49">
         <f>SUM(F10:F34)</f>
@@ -4844,19 +4862,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="134" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="133"/>
-      <c r="C1" s="133"/>
-      <c r="D1" s="133"/>
-      <c r="E1" s="133"/>
-      <c r="F1" s="133"/>
-      <c r="G1" s="133"/>
-      <c r="H1" s="133"/>
-      <c r="I1" s="133"/>
-      <c r="J1" s="133"/>
-      <c r="K1" s="133"/>
+      <c r="B1" s="134"/>
+      <c r="C1" s="134"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="134"/>
+      <c r="J1" s="134"/>
+      <c r="K1" s="134"/>
     </row>
     <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="73" t="s">
@@ -5520,16 +5538,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="131" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E2" s="36"/>
@@ -6305,71 +6323,71 @@
       <c r="A21" s="96" t="s">
         <v>159</v>
       </c>
-      <c r="B21" s="135" t="s">
+      <c r="B21" s="136" t="s">
         <v>187</v>
       </c>
-      <c r="C21" s="135"/>
-      <c r="D21" s="135"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="136"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="101" t="s">
         <v>178</v>
       </c>
-      <c r="B22" s="136" t="s">
+      <c r="B22" s="137" t="s">
         <v>188</v>
       </c>
-      <c r="C22" s="136"/>
-      <c r="D22" s="136"/>
+      <c r="C22" s="137"/>
+      <c r="D22" s="137"/>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="101" t="s">
         <v>189</v>
       </c>
-      <c r="B23" s="136" t="s">
+      <c r="B23" s="137" t="s">
         <v>190</v>
       </c>
-      <c r="C23" s="136"/>
-      <c r="D23" s="136"/>
+      <c r="C23" s="137"/>
+      <c r="D23" s="137"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="101" t="s">
         <v>191</v>
       </c>
-      <c r="B24" s="136" t="s">
+      <c r="B24" s="137" t="s">
         <v>192</v>
       </c>
-      <c r="C24" s="136"/>
-      <c r="D24" s="136"/>
+      <c r="C24" s="137"/>
+      <c r="D24" s="137"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="98"/>
-      <c r="B25" s="134"/>
-      <c r="C25" s="134"/>
-      <c r="D25" s="134"/>
+      <c r="B25" s="135"/>
+      <c r="C25" s="135"/>
+      <c r="D25" s="135"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="98"/>
-      <c r="B26" s="134"/>
-      <c r="C26" s="134"/>
-      <c r="D26" s="134"/>
+      <c r="B26" s="135"/>
+      <c r="C26" s="135"/>
+      <c r="D26" s="135"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="98"/>
-      <c r="B27" s="134"/>
-      <c r="C27" s="134"/>
-      <c r="D27" s="134"/>
+      <c r="B27" s="135"/>
+      <c r="C27" s="135"/>
+      <c r="D27" s="135"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="98"/>
-      <c r="B28" s="134"/>
-      <c r="C28" s="134"/>
-      <c r="D28" s="134"/>
+      <c r="B28" s="135"/>
+      <c r="C28" s="135"/>
+      <c r="D28" s="135"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="98"/>
-      <c r="B29" s="134"/>
-      <c r="C29" s="134"/>
-      <c r="D29" s="134"/>
+      <c r="B29" s="135"/>
+      <c r="C29" s="135"/>
+      <c r="D29" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>